<commit_message>
It appears BooleanDetector is 5min off at end of pass
</commit_message>
<xml_diff>
--- a/OrekitAccessDopplerCalculator/TLEaccessResultsAfter1DayUpdate.xlsx
+++ b/OrekitAccessDopplerCalculator/TLEaccessResultsAfter1DayUpdate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\MSD\Java Code\FeasibilityStudies\OrekitAccessDopplerCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96BAD5B-54F9-4C43-861B-3BF79C19FF92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8648524B-BB12-40D5-B8BE-B4D9EB614B19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED4432F7-8988-4CDC-90ED-592CB974EBBD}"/>
+    <workbookView xWindow="17685" yWindow="1920" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{ED4432F7-8988-4CDC-90ED-592CB974EBBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,12 +562,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -575,7 +575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -583,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -591,7 +591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -599,7 +599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -607,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -615,7 +615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -623,7 +623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -631,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -639,7 +639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -647,7 +647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -668,13 +668,13 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -682,7 +682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43853.327046863429</v>
       </c>
@@ -693,7 +693,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43853.32789158565</v>
       </c>
@@ -704,7 +704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43853.392169733794</v>
       </c>
@@ -715,7 +715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43853.39861527778</v>
       </c>
@@ -726,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43853.459848229169</v>
       </c>
@@ -737,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43853.467252951392</v>
       </c>
@@ -748,7 +748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43853.52810920139</v>
       </c>
@@ -759,7 +759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43853.535501886574</v>
       </c>
@@ -770,7 +770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43853.596766759256</v>
       </c>
@@ -781,7 +781,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43853.60314540509</v>
       </c>
@@ -792,164 +792,164 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -968,13 +968,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -982,7 +982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>